<commit_message>
WebResource, progress bar and new functionalities were added
Multiple updates were made by the help of Erduran KORKUT
</commit_message>
<xml_diff>
--- a/EntityCreator/Resources/Template.xlsx
+++ b/EntityCreator/Resources/Template.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="6750" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Entity" sheetId="1" r:id="rId1"/>
+    <sheet name="WebResource" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t>LogicalName</t>
   </si>
@@ -170,6 +171,21 @@
   </si>
   <si>
     <t>true;false</t>
+  </si>
+  <si>
+    <t>Logical Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Ex. Attr. 12</t>
+  </si>
+  <si>
+    <t>Float</t>
   </si>
 </sst>
 </file>
@@ -530,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,8 +814,56 @@
         <v>2000</v>
       </c>
     </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Leak, Processbar Fixes and NN Relation Updates
Memory leak issue fixed.
Process bar removed, current item info added.
NN relation creation added.
</commit_message>
<xml_diff>
--- a/EntityCreator/Resources/Template.xlsx
+++ b/EntityCreator/Resources/Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6750" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="7680" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Entity" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
   <si>
     <t>LogicalName</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Example Attribute Description</t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
@@ -186,6 +183,27 @@
   </si>
   <si>
     <t>Float</t>
+  </si>
+  <si>
+    <t>IsRequired</t>
+  </si>
+  <si>
+    <t>pfx_exampleattr12</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>pfx_exampleattr13</t>
+  </si>
+  <si>
+    <t>Ex. Attr. 13</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>SingleLine</t>
   </si>
 </sst>
 </file>
@@ -546,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,9 +581,10 @@
     <col min="7" max="7" width="30.7109375" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,7 +598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -595,7 +614,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,16 +634,19 @@
         <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -635,24 +657,27 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="I4">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
       <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -661,18 +686,18 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -680,149 +705,175 @@
       <c r="I6">
         <v>1000000</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>50</v>
       </c>
-      <c r="G8" t="s">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>44</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
         <v>45</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
       </c>
       <c r="I14">
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
       <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s">
-        <v>56</v>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -848,7 +899,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -857,10 +908,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>